<commit_message>
update more sample points
</commit_message>
<xml_diff>
--- a/applets/level_curves/evaluation/output.xlsx
+++ b/applets/level_curves/evaluation/output.xlsx
@@ -522,19 +522,19 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F3" t="n">
         <v>45</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.711</t>
+          <t>0.867</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[(0, 43), (1, 1), (2, 2), (3, 3), (4, 4), (5, 37), (6, 6), (7, 7), (8, 8), (9, 5), (10, 5), (11, 11), (12, 12), (13, 13), (14, 2), (15, 15), (16, 16), (17, 17), (18, 43), (19, 26), (20, 20), (21, 21), (22, 22), (23, 23), (24, 30), (25, 25), (26, 26), (27, 27), (28, 28), (29, 8), (30, 30), (31, 8), (32, 32), (33, 33), (34, 34), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39), (40, 43), (41, 6), (42, 42), (43, 41), (44, 44)]</t>
+          <t>[(0, 5), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 15), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 15), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25), (26, 7), (27, 27), (28, 28), (29, 29), (30, 30), (31, 31), (32, 32), (33, 33), (34, 34), (35, 35), (36, 36), (37, 31), (38, 38), (39, 39), (40, 40), (41, 41), (42, 42), (43, 25), (44, 44)]</t>
         </is>
       </c>
     </row>
@@ -556,19 +556,19 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F4" t="n">
         <v>45</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.622</t>
+          <t>0.756</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 6), (3, 8), (4, 4), (5, 35), (6, 6), (7, 7), (8, 8), (9, 5), (10, 5), (11, 35), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 5), (19, 43), (20, 43), (21, 21), (22, 6), (23, 23), (24, 5), (25, 25), (26, 43), (27, 27), (28, 28), (29, 8), (30, 30), (31, 31), (32, 41), (33, 8), (34, 34), (35, 35), (36, 41), (37, 37), (38, 38), (39, 39), (40, 40), (41, 2), (42, 42), (43, 43), (44, 44)]</t>
+          <t>[(0, 35), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 25), (10, 10), (11, 15), (12, 15), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 25), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25), (26, 40), (27, 27), (28, 28), (29, 29), (30, 30), (31, 31), (32, 32), (33, 5), (34, 34), (35, 35), (36, 10), (37, 15), (38, 38), (39, 39), (40, 40), (41, 5), (42, 42), (43, 25), (44, 44)]</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[(0, 43), (1, 37), (2, 2), (3, 43), (4, 6), (5, 35), (6, 37), (7, 7), (8, 6), (9, 35), (10, 38), (11, 43), (12, 12), (13, 13), (14, 44), (15, 15), (16, 16), (17, 35), (18, 43), (19, 43), (20, 43), (21, 21), (22, 22), (23, 23), (24, 26), (25, 35), (26, 37), (27, 27), (28, 28), (29, 2), (30, 30), (31, 31), (32, 37), (33, 27), (34, 0), (35, 35), (36, 2), (37, 37), (38, 21), (39, 12), (40, 8), (41, 41), (42, 43), (43, 43), (44, 44)]</t>
+          <t>[(0, 5), (1, 15), (2, 2), (3, 10), (4, 25), (5, 5), (6, 15), (7, 15), (8, 8), (9, 15), (10, 35), (11, 15), (12, 15), (13, 29), (14, 2), (15, 15), (16, 16), (17, 17), (18, 25), (19, 15), (20, 20), (21, 21), (22, 22), (23, 25), (24, 15), (25, 25), (26, 5), (27, 27), (28, 28), (29, 29), (30, 30), (31, 31), (32, 25), (33, 5), (34, 34), (35, 35), (36, 25), (37, 15), (38, 25), (39, 5), (40, 40), (41, 5), (42, 5), (43, 25), (44, 25)]</t>
         </is>
       </c>
     </row>
@@ -624,19 +624,19 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F6" t="n">
         <v>45</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.222</t>
+          <t>0.356</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[(0, 5), (1, 7), (2, 27), (3, 7), (4, 35), (5, 2), (6, 37), (7, 6), (8, 2), (9, 6), (10, 27), (11, 35), (12, 30), (13, 13), (14, 44), (15, 35), (16, 6), (17, 37), (18, 8), (19, 26), (20, 27), (21, 21), (22, 22), (23, 37), (24, 38), (25, 25), (26, 37), (27, 37), (28, 28), (29, 35), (30, 37), (31, 27), (32, 37), (33, 27), (34, 37), (35, 35), (36, 36), (37, 37), (38, 38), (39, 44), (40, 30), (41, 37), (42, 38), (43, 5), (44, 44)]</t>
+          <t>[(0, 43), (1, 5), (2, 10), (3, 10), (4, 4), (5, 5), (6, 6), (7, 25), (8, 15), (9, 15), (10, 27), (11, 10), (12, 10), (13, 6), (14, 5), (15, 15), (16, 16), (17, 17), (18, 25), (19, 15), (20, 20), (21, 21), (22, 22), (23, 39), (24, 24), (25, 25), (26, 15), (27, 15), (28, 15), (29, 15), (30, 25), (31, 17), (32, 17), (33, 8), (34, 34), (35, 35), (36, 10), (37, 7), (38, 25), (39, 25), (40, 40), (41, 5), (42, 25), (43, 43), (44, 44)]</t>
         </is>
       </c>
     </row>
@@ -658,19 +658,19 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>45</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.067</t>
+          <t>0.044</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[(0, 44), (1, 35), (2, 2), (3, 5), (4, 35), (5, 35), (6, 44), (7, 37), (8, 17), (9, 37), (10, 35), (11, 37), (12, 37), (13, 13), (14, 37), (15, 35), (16, 5), (17, 35), (18, 37), (19, 43), (20, 37), (21, 35), (22, 38), (23, 35), (24, 27), (25, 37), (26, 37), (27, 37), (28, 0), (29, 5), (30, 27), (31, 44), (32, 32), (33, 30), (34, 35), (35, 37), (36, 27), (37, 27), (38, 27), (39, 13), (40, 35), (41, 37), (42, 35), (43, 37), (44, 13)]</t>
+          <t>[(0, 15), (1, 25), (2, 25), (3, 31), (4, 15), (5, 25), (6, 27), (7, 5), (8, 35), (9, 17), (10, 25), (11, 15), (12, 25), (13, 31), (14, 25), (15, 25), (16, 15), (17, 25), (18, 25), (19, 25), (20, 35), (21, 29), (22, 25), (23, 28), (24, 25), (25, 25), (26, 10), (27, 10), (28, 10), (29, 29), (30, 25), (31, 35), (32, 25), (33, 5), (34, 10), (35, 17), (36, 25), (37, 39), (38, 29), (39, 17), (40, 15), (41, 5), (42, 25), (43, 25), (44, 17)]</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[(0, 16), (1, 3), (2, 2), (3, 3), (4, 11), (5, 5), (6, 6), (7, 14), (8, 8), (9, 11), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 14), (17, 14), (18, 18), (19, 11), (20, 20), (21, 21), (22, 22), (23, 23), (24, 25), (25, 25)]</t>
+          <t>[(0, 14), (1, 1), (2, 2), (3, 3), (4, 14), (5, 5), (6, 14), (7, 14), (8, 8), (9, 9), (10, 10), (11, 14), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 14), (21, 14), (22, 25), (23, 23), (24, 14), (25, 25)]</t>
         </is>
       </c>
     </row>
@@ -760,19 +760,19 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" t="n">
         <v>26</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.462</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[(0, 16), (1, 1), (2, 2), (3, 3), (4, 25), (5, 5), (6, 25), (7, 14), (8, 8), (9, 14), (10, 10), (11, 14), (12, 7), (13, 13), (14, 14), (15, 25), (16, 16), (17, 14), (18, 18), (19, 19), (20, 20), (21, 14), (22, 14), (23, 23), (24, 7), (25, 8)]</t>
+          <t>[(0, 14), (1, 1), (2, 2), (3, 3), (4, 4), (5, 14), (6, 14), (7, 14), (8, 8), (9, 25), (10, 14), (11, 14), (12, 12), (13, 14), (14, 14), (15, 15), (16, 16), (17, 14), (18, 14), (19, 19), (20, 20), (21, 25), (22, 22), (23, 14), (24, 14), (25, 14)]</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 25), (2, 25), (3, 3), (4, 14), (5, 11), (6, 14), (7, 14), (8, 8), (9, 14), (10, 10), (11, 11), (12, 7), (13, 25), (14, 14), (15, 25), (16, 16), (17, 14), (18, 8), (19, 11), (20, 14), (21, 25), (22, 14), (23, 14), (24, 25), (25, 25)]</t>
+          <t>[(0, 14), (1, 1), (2, 14), (3, 14), (4, 4), (5, 20), (6, 14), (7, 14), (8, 14), (9, 14), (10, 10), (11, 14), (12, 12), (13, 14), (14, 14), (15, 14), (16, 16), (17, 14), (18, 14), (19, 14), (20, 14), (21, 14), (22, 14), (23, 14), (24, 14), (25, 25)]</t>
         </is>
       </c>
     </row>
@@ -828,19 +828,19 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>26</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.115</t>
+          <t>0.077</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 7), (2, 25), (3, 8), (4, 20), (5, 14), (6, 7), (7, 14), (8, 8), (9, 7), (10, 11), (11, 8), (12, 25), (13, 14), (14, 14), (15, 7), (16, 14), (17, 14), (18, 20), (19, 19), (20, 14), (21, 8), (22, 14), (23, 3), (24, 20), (25, 11)]</t>
+          <t>[(0, 14), (1, 14), (2, 14), (3, 14), (4, 14), (5, 14), (6, 14), (7, 14), (8, 14), (9, 14), (10, 14), (11, 14), (12, 14), (13, 14), (14, 14), (15, 3), (16, 14), (17, 14), (18, 14), (19, 14), (20, 14), (21, 14), (22, 22), (23, 14), (24, 14), (25, 14)]</t>
         </is>
       </c>
     </row>
@@ -862,19 +862,19 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>26</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.115</t>
+          <t>0.038</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 14), (2, 14), (3, 8), (4, 20), (5, 14), (6, 11), (7, 20), (8, 8), (9, 14), (10, 4), (11, 20), (12, 8), (13, 14), (14, 14), (15, 20), (16, 14), (17, 20), (18, 8), (19, 11), (20, 20), (21, 8), (22, 14), (23, 11), (24, 14), (25, 20)]</t>
+          <t>[(0, 14), (1, 14), (2, 14), (3, 14), (4, 14), (5, 14), (6, 14), (7, 14), (8, 14), (9, 14), (10, 14), (11, 14), (12, 14), (13, 14), (14, 14), (15, 14), (16, 14), (17, 14), (18, 14), (19, 14), (20, 14), (21, 14), (22, 14), (23, 14), (24, 14), (25, 14)]</t>
         </is>
       </c>
     </row>
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>11</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.818</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>[(0, 5), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 5), (8, 8), (9, 9), (10, 10)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 6), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10)]</t>
         </is>
       </c>
     </row>
@@ -964,19 +964,19 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>11</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.545</t>
+          <t>0.727</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 5), (3, 3), (4, 3), (5, 10), (6, 6), (7, 3), (8, 5), (9, 9), (10, 10)]</t>
+          <t>[(0, 3), (1, 1), (2, 2), (3, 3), (4, 4), (5, 6), (6, 6), (7, 6), (8, 8), (9, 9), (10, 10)]</t>
         </is>
       </c>
     </row>
@@ -998,19 +998,19 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>11</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.818</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>[(0, 10), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 3), (8, 8), (9, 9), (10, 10)]</t>
+          <t>[(0, 10), (1, 1), (2, 2), (3, 3), (4, 4), (5, 6), (6, 6), (7, 6), (8, 8), (9, 9), (10, 9)]</t>
         </is>
       </c>
     </row>
@@ -1032,19 +1032,19 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>11</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.182</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>[(0, 2), (1, 2), (2, 3), (3, 5), (4, 2), (5, 5), (6, 10), (7, 3), (8, 10), (9, 9), (10, 6)]</t>
+          <t>[(0, 0), (1, 1), (2, 9), (3, 3), (4, 9), (5, 5), (6, 6), (7, 6), (8, 3), (9, 9), (10, 10)]</t>
         </is>
       </c>
     </row>
@@ -1066,19 +1066,19 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>11</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.364</t>
+          <t>0.091</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 3), (2, 5), (3, 10), (4, 5), (5, 5), (6, 6), (7, 5), (8, 5), (9, 9), (10, 5)]</t>
+          <t>[(0, 6), (1, 6), (2, 6), (3, 6), (4, 10), (5, 9), (6, 9), (7, 9), (8, 9), (9, 9), (10, 4)]</t>
         </is>
       </c>
     </row>
@@ -1134,19 +1134,19 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F21" t="n">
         <v>30</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.967</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>[(0, 1), (1, 1), (2, 26), (3, 3), (4, 4), (5, 6), (6, 6), (7, 26), (8, 4), (9, 29), (10, 26), (11, 11), (12, 19), (13, 13), (14, 14), (15, 6), (16, 16), (17, 17), (18, 18), (19, 29), (20, 20), (21, 21), (22, 17), (23, 23), (24, 29), (25, 16), (26, 29), (27, 27), (28, 23), (29, 29)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 1), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25), (26, 26), (27, 27), (28, 28), (29, 29)]</t>
         </is>
       </c>
     </row>
@@ -1168,19 +1168,19 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F22" t="n">
         <v>30</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>[(0, 22), (1, 1), (2, 26), (3, 16), (4, 4), (5, 5), (6, 6), (7, 26), (8, 16), (9, 29), (10, 10), (11, 11), (12, 19), (13, 13), (14, 26), (15, 29), (16, 23), (17, 17), (18, 18), (19, 29), (20, 20), (21, 21), (22, 29), (23, 23), (24, 24), (25, 16), (26, 26), (27, 26), (28, 29), (29, 29)]</t>
+          <t>[(0, 0), (1, 1), (2, 23), (3, 17), (4, 4), (5, 5), (6, 6), (7, 23), (8, 23), (9, 23), (10, 10), (11, 23), (12, 12), (13, 24), (14, 23), (15, 15), (16, 16), (17, 17), (18, 17), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25), (26, 26), (27, 27), (28, 28), (29, 29)]</t>
         </is>
       </c>
     </row>
@@ -1202,19 +1202,19 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F23" t="n">
         <v>30</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.267</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>[(0, 22), (1, 1), (2, 29), (3, 29), (4, 19), (5, 5), (6, 26), (7, 26), (8, 9), (9, 19), (10, 1), (11, 6), (12, 24), (13, 13), (14, 16), (15, 29), (16, 16), (17, 17), (18, 29), (19, 29), (20, 20), (21, 29), (22, 26), (23, 11), (24, 29), (25, 16), (26, 26), (27, 26), (28, 6), (29, 29)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 23), (4, 29), (5, 5), (6, 6), (7, 26), (8, 8), (9, 23), (10, 10), (11, 17), (12, 23), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 23), (19, 19), (20, 20), (21, 17), (22, 23), (23, 23), (24, 24), (25, 25), (26, 26), (27, 27), (28, 17), (29, 29)]</t>
         </is>
       </c>
     </row>
@@ -1236,19 +1236,19 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>30</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.233</t>
+          <t>0.267</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>[(0, 17), (1, 1), (2, 29), (3, 6), (4, 19), (5, 23), (6, 6), (7, 26), (8, 19), (9, 29), (10, 26), (11, 29), (12, 16), (13, 11), (14, 16), (15, 15), (16, 16), (17, 17), (18, 16), (19, 29), (20, 6), (21, 29), (22, 6), (23, 11), (24, 13), (25, 29), (26, 26), (27, 29), (28, 6), (29, 29)]</t>
+          <t>[(0, 0), (1, 1), (2, 23), (3, 25), (4, 17), (5, 29), (6, 17), (7, 25), (8, 17), (9, 7), (10, 26), (11, 17), (12, 17), (13, 29), (14, 23), (15, 17), (16, 16), (17, 17), (18, 13), (19, 22), (20, 20), (21, 17), (22, 17), (23, 23), (24, 19), (25, 25), (26, 26), (27, 23), (28, 17), (29, 17)]</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>[(0, 29), (1, 29), (2, 11), (3, 29), (4, 5), (5, 26), (6, 6), (7, 29), (8, 29), (9, 11), (10, 1), (11, 6), (12, 19), (13, 29), (14, 23), (15, 26), (16, 6), (17, 28), (18, 16), (19, 29), (20, 29), (21, 26), (22, 29), (23, 9), (24, 26), (25, 16), (26, 29), (27, 19), (28, 6), (29, 29)]</t>
+          <t>[(0, 1), (1, 1), (2, 19), (3, 23), (4, 29), (5, 23), (6, 23), (7, 25), (8, 22), (9, 17), (10, 19), (11, 17), (12, 23), (13, 29), (14, 23), (15, 19), (16, 23), (17, 23), (18, 1), (19, 23), (20, 23), (21, 23), (22, 22), (23, 17), (24, 13), (25, 19), (26, 23), (27, 23), (28, 17), (29, 22)]</t>
         </is>
       </c>
     </row>
@@ -1338,19 +1338,19 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F27" t="n">
         <v>16</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 12), (3, 3), (4, 1), (5, 11), (6, 1), (7, 11), (8, 1), (9, 1), (10, 10), (11, 11), (12, 12), (13, 13), (14, 12), (15, 15)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 1), (10, 10), (11, 11), (12, 12), (13, 13), (14, 1), (15, 15)]</t>
         </is>
       </c>
     </row>
@@ -1372,19 +1372,19 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F28" t="n">
         <v>16</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.562</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 1), (3, 1), (4, 11), (5, 11), (6, 1), (7, 1), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 3), (15, 15)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 1), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15)]</t>
         </is>
       </c>
     </row>
@@ -1406,19 +1406,19 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>16</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.562</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 12), (3, 1), (4, 0), (5, 11), (6, 11), (7, 0), (8, 1), (9, 11), (10, 11), (11, 11), (12, 1), (13, 13), (14, 13), (15, 1)]</t>
+          <t>[(0, 0), (1, 1), (2, 10), (3, 1), (4, 1), (5, 1), (6, 10), (7, 1), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 1)]</t>
         </is>
       </c>
     </row>
@@ -1440,19 +1440,19 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>16</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.312</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 11), (2, 1), (3, 1), (4, 1), (5, 0), (6, 1), (7, 0), (8, 11), (9, 11), (10, 15), (11, 11), (12, 11), (13, 0), (14, 1), (15, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 1), (3, 1), (4, 1), (5, 5), (6, 12), (7, 1), (8, 1), (9, 1), (10, 10), (11, 1), (12, 12), (13, 0), (14, 1), (15, 1)]</t>
         </is>
       </c>
     </row>
@@ -1474,19 +1474,19 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
         <v>16</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0.188</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 1), (3, 3), (4, 0), (5, 0), (6, 1), (7, 15), (8, 0), (9, 1), (10, 11), (11, 0), (12, 11), (13, 1), (14, 11), (15, 0)]</t>
+          <t>[(0, 1), (1, 0), (2, 1), (3, 10), (4, 11), (5, 1), (6, 1), (7, 1), (8, 10), (9, 1), (10, 1), (11, 1), (12, 1), (13, 1), (14, 1), (15, 1)]</t>
         </is>
       </c>
     </row>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 4), (3, 3), (4, 4), (5, 5), (6, 6)]</t>
+          <t>[(0, 0), (1, 1), (2, 5), (3, 3), (4, 4), (5, 5), (6, 6)]</t>
         </is>
       </c>
     </row>
@@ -1576,19 +1576,19 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>7</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>0.714</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 5), (3, 4), (4, 4), (5, 5), (6, 6)]</t>
+          <t>[(0, 0), (1, 1), (2, 5), (3, 3), (4, 4), (5, 5), (6, 6)]</t>
         </is>
       </c>
     </row>
@@ -1610,19 +1610,19 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>7</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0.714</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>[(0, 5), (1, 1), (2, 5), (3, 3), (4, 4), (5, 5), (6, 6)]</t>
+          <t>[(0, 0), (1, 0), (2, 5), (3, 3), (4, 5), (5, 5), (6, 5)]</t>
         </is>
       </c>
     </row>
@@ -1644,19 +1644,19 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36" t="n">
         <v>7</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.429</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 5), (2, 5), (3, 6), (4, 4), (5, 5), (6, 5)]</t>
+          <t>[(0, 0), (1, 1), (2, 5), (3, 5), (4, 4), (5, 5), (6, 0)]</t>
         </is>
       </c>
     </row>
@@ -1678,19 +1678,19 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>7</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.286</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[(0, 5), (1, 5), (2, 5), (3, 5), (4, 4), (5, 5), (6, 5)]</t>
+          <t>[(0, 0), (1, 1), (2, 0), (3, 0), (4, 0), (5, 5), (6, 0)]</t>
         </is>
       </c>
     </row>
@@ -1746,19 +1746,19 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="F39" t="n">
         <v>40</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>0.400</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>[(0, 2), (1, 2), (2, 2), (3, 3), (4, 23), (5, 2), (6, 10), (7, 23), (8, 8), (9, 23), (10, 10), (11, 3), (12, 12), (13, 10), (14, 2), (15, 23), (16, 2), (17, 17), (18, 8), (19, 19), (20, 23), (21, 21), (22, 2), (23, 23), (24, 23), (25, 25), (26, 10), (27, 10), (28, 39), (29, 29), (30, 10), (31, 2), (32, 32), (33, 33), (34, 34), (35, 12), (36, 34), (37, 37), (38, 2), (39, 39)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 0), (7, 26), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 10), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 0), (25, 25), (26, 26), (27, 27), (28, 28), (29, 29), (30, 30), (31, 31), (32, 32), (33, 33), (34, 34), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39)]</t>
         </is>
       </c>
     </row>
@@ -1780,19 +1780,19 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F40" t="n">
         <v>40</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>0.300</t>
+          <t>0.725</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>[(0, 12), (1, 2), (2, 2), (3, 3), (4, 23), (5, 5), (6, 23), (7, 23), (8, 8), (9, 9), (10, 10), (11, 23), (12, 23), (13, 10), (14, 2), (15, 21), (16, 16), (17, 17), (18, 12), (19, 19), (20, 21), (21, 5), (22, 5), (23, 2), (24, 30), (25, 2), (26, 10), (27, 21), (28, 10), (29, 29), (30, 10), (31, 10), (32, 32), (33, 33), (34, 39), (35, 32), (36, 23), (37, 20), (38, 2), (39, 2)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 10), (6, 23), (7, 12), (8, 8), (9, 9), (10, 10), (11, 26), (12, 12), (13, 13), (14, 5), (15, 15), (16, 16), (17, 10), (18, 18), (19, 19), (20, 20), (21, 21), (22, 18), (23, 23), (24, 33), (25, 25), (26, 26), (27, 23), (28, 26), (29, 29), (30, 30), (31, 31), (32, 32), (33, 33), (34, 10), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39)]</t>
         </is>
       </c>
     </row>
@@ -1814,19 +1814,19 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F41" t="n">
         <v>40</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>[(0, 23), (1, 1), (2, 2), (3, 2), (4, 2), (5, 5), (6, 10), (7, 23), (8, 8), (9, 5), (10, 10), (11, 2), (12, 23), (13, 19), (14, 39), (15, 23), (16, 2), (17, 2), (18, 8), (19, 19), (20, 2), (21, 2), (22, 22), (23, 23), (24, 30), (25, 2), (26, 2), (27, 32), (28, 39), (29, 29), (30, 10), (31, 10), (32, 2), (33, 2), (34, 3), (35, 8), (36, 23), (37, 2), (38, 2), (39, 39)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 23), (5, 5), (6, 6), (7, 5), (8, 8), (9, 10), (10, 10), (11, 10), (12, 12), (13, 12), (14, 10), (15, 15), (16, 15), (17, 10), (18, 8), (19, 19), (20, 23), (21, 21), (22, 23), (23, 23), (24, 8), (25, 23), (26, 23), (27, 23), (28, 28), (29, 29), (30, 8), (31, 17), (32, 8), (33, 33), (34, 34), (35, 35), (36, 36), (37, 8), (38, 23), (39, 39)]</t>
         </is>
       </c>
     </row>
@@ -1848,19 +1848,19 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
         <v>40</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0.175</t>
+          <t>0.250</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>[(0, 2), (1, 2), (2, 2), (3, 12), (4, 8), (5, 5), (6, 10), (7, 2), (8, 8), (9, 23), (10, 10), (11, 39), (12, 10), (13, 23), (14, 2), (15, 23), (16, 2), (17, 8), (18, 2), (19, 1), (20, 2), (21, 2), (22, 39), (23, 2), (24, 15), (25, 2), (26, 2), (27, 2), (28, 2), (29, 29), (30, 30), (31, 2), (32, 2), (33, 5), (34, 2), (35, 2), (36, 39), (37, 30), (38, 2), (39, 39)]</t>
+          <t>[(0, 10), (1, 10), (2, 10), (3, 8), (4, 10), (5, 10), (6, 24), (7, 10), (8, 8), (9, 12), (10, 10), (11, 10), (12, 12), (13, 10), (14, 10), (15, 10), (16, 16), (17, 8), (18, 2), (19, 19), (20, 0), (21, 21), (22, 19), (23, 23), (24, 0), (25, 12), (26, 8), (27, 27), (28, 23), (29, 10), (30, 10), (31, 10), (32, 23), (33, 23), (34, 23), (35, 33), (36, 10), (37, 37), (38, 0), (39, 39)]</t>
         </is>
       </c>
     </row>
@@ -1882,19 +1882,19 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>40</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0.050</t>
+          <t>0.075</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>[(0, 3), (1, 10), (2, 29), (3, 2), (4, 39), (5, 2), (6, 5), (7, 2), (8, 37), (9, 30), (10, 29), (11, 2), (12, 2), (13, 2), (14, 2), (15, 2), (16, 15), (17, 2), (18, 29), (19, 2), (20, 2), (21, 2), (22, 30), (23, 23), (24, 23), (25, 2), (26, 2), (27, 10), (28, 39), (29, 2), (30, 6), (31, 10), (32, 29), (33, 29), (34, 2), (35, 8), (36, 1), (37, 39), (38, 23), (39, 39)]</t>
+          <t>[(0, 23), (1, 10), (2, 9), (3, 3), (4, 8), (5, 23), (6, 23), (7, 26), (8, 8), (9, 10), (10, 23), (11, 23), (12, 23), (13, 8), (14, 23), (15, 10), (16, 23), (17, 8), (18, 10), (19, 23), (20, 23), (21, 10), (22, 10), (23, 23), (24, 23), (25, 23), (26, 10), (27, 23), (28, 10), (29, 33), (30, 3), (31, 23), (32, 23), (33, 23), (34, 19), (35, 23), (36, 8), (37, 8), (38, 10), (39, 10)]</t>
         </is>
       </c>
     </row>
@@ -1950,19 +1950,19 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F45" t="n">
         <v>15</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>0.467</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>[(0, 7), (1, 7), (2, 7), (3, 3), (4, 1), (5, 5), (6, 6), (7, 7), (8, 8), (9, 8), (10, 10), (11, 7), (12, 7), (13, 7), (14, 14)]</t>
+          <t>[(0, 8), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14)]</t>
         </is>
       </c>
     </row>
@@ -1984,19 +1984,19 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F46" t="n">
         <v>15</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0.733</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 3), (6, 6), (7, 7), (8, 8), (9, 1), (10, 10), (11, 5), (12, 12), (13, 13), (14, 7)]</t>
+          <t>[(0, 0), (1, 7), (2, 2), (3, 3), (4, 4), (5, 7), (6, 6), (7, 7), (8, 8), (9, 7), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14)]</t>
         </is>
       </c>
     </row>
@@ -2018,19 +2018,19 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>15</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.600</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 7), (2, 7), (3, 3), (4, 4), (5, 5), (6, 6), (7, 3), (8, 7), (9, 13), (10, 7), (11, 7), (12, 7), (13, 13), (14, 7)]</t>
+          <t>[(0, 12), (1, 7), (2, 7), (3, 7), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 12), (10, 10), (11, 11), (12, 12), (13, 6), (14, 14)]</t>
         </is>
       </c>
     </row>
@@ -2052,19 +2052,19 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>15</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.200</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 8), (2, 7), (3, 3), (4, 7), (5, 5), (6, 6), (7, 5), (8, 8), (9, 13), (10, 7), (11, 5), (12, 7), (13, 13), (14, 7)]</t>
+          <t>[(0, 6), (1, 7), (2, 12), (3, 7), (4, 7), (5, 5), (6, 6), (7, 3), (8, 12), (9, 7), (10, 7), (11, 7), (12, 12), (13, 7), (14, 7)]</t>
         </is>
       </c>
     </row>
@@ -2086,19 +2086,19 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>15</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>0.133</t>
+          <t>0.200</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>[(0, 3), (1, 5), (2, 3), (3, 3), (4, 3), (5, 5), (6, 5), (7, 3), (8, 5), (9, 7), (10, 14), (11, 5), (12, 7), (13, 3), (14, 3)]</t>
+          <t>[(0, 12), (1, 7), (2, 5), (3, 12), (4, 7), (5, 11), (6, 6), (7, 7), (8, 8), (9, 12), (10, 5), (11, 7), (12, 7), (13, 7), (14, 7)]</t>
         </is>
       </c>
     </row>
@@ -2154,19 +2154,19 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F51" t="n">
         <v>25</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 4), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 19), (24, 10)]</t>
+          <t>[(0, 19), (1, 1), (2, 2), (3, 3), (4, 19), (5, 5), (6, 6), (7, 7), (8, 8), (9, 23), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 19), (17, 19), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
         </is>
       </c>
     </row>
@@ -2188,19 +2188,19 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
         <v>25</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>0.480</t>
+          <t>0.400</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 10), (2, 2), (3, 21), (4, 4), (5, 5), (6, 12), (7, 15), (8, 4), (9, 12), (10, 10), (11, 19), (12, 21), (13, 21), (14, 21), (15, 15), (16, 16), (17, 19), (18, 10), (19, 19), (20, 20), (21, 21), (22, 22), (23, 21), (24, 24)]</t>
+          <t>[(0, 0), (1, 10), (2, 2), (3, 19), (4, 3), (5, 19), (6, 6), (7, 19), (8, 8), (9, 1), (10, 10), (11, 11), (12, 2), (13, 2), (14, 1), (15, 15), (16, 19), (17, 19), (18, 18), (19, 19), (20, 20), (21, 12), (22, 19), (23, 19), (24, 19)]</t>
         </is>
       </c>
     </row>
@@ -2222,19 +2222,19 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>25</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>0.320</t>
+          <t>0.360</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>[(0, 21), (1, 10), (2, 15), (3, 21), (4, 4), (5, 5), (6, 3), (7, 21), (8, 8), (9, 21), (10, 10), (11, 19), (12, 19), (13, 10), (14, 22), (15, 10), (16, 21), (17, 21), (18, 10), (19, 19), (20, 20), (21, 21), (22, 22), (23, 10), (24, 12)]</t>
+          <t>[(0, 0), (1, 19), (2, 2), (3, 19), (4, 1), (5, 5), (6, 19), (7, 19), (8, 8), (9, 1), (10, 2), (11, 11), (12, 1), (13, 5), (14, 19), (15, 19), (16, 19), (17, 19), (18, 18), (19, 19), (20, 19), (21, 21), (22, 22), (23, 19), (24, 1)]</t>
         </is>
       </c>
     </row>
@@ -2256,19 +2256,19 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>25</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>0.120</t>
+          <t>0.080</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>[(0, 21), (1, 20), (2, 15), (3, 3), (4, 2), (5, 22), (6, 4), (7, 20), (8, 10), (9, 15), (10, 10), (11, 4), (12, 12), (13, 22), (14, 22), (15, 10), (16, 10), (17, 4), (18, 21), (19, 21), (20, 21), (21, 20), (22, 10), (23, 22), (24, 10)]</t>
+          <t>[(0, 0), (1, 2), (2, 19), (3, 18), (4, 5), (5, 5), (6, 19), (7, 19), (8, 7), (9, 1), (10, 19), (11, 19), (12, 2), (13, 19), (14, 10), (15, 19), (16, 6), (17, 19), (18, 19), (19, 1), (20, 19), (21, 10), (22, 2), (23, 5), (24, 19)]</t>
         </is>
       </c>
     </row>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>[(0, 20), (1, 10), (2, 22), (3, 20), (4, 20), (5, 22), (6, 21), (7, 21), (8, 22), (9, 20), (10, 22), (11, 21), (12, 21), (13, 21), (14, 20), (15, 15), (16, 10), (17, 20), (18, 22), (19, 20), (20, 20), (21, 20), (22, 20), (23, 20), (24, 20)]</t>
+          <t>[(0, 19), (1, 1), (2, 5), (3, 19), (4, 19), (5, 19), (6, 19), (7, 19), (8, 1), (9, 19), (10, 19), (11, 11), (12, 10), (13, 2), (14, 2), (15, 0), (16, 5), (17, 1), (18, 2), (19, 24), (20, 5), (21, 19), (22, 11), (23, 1), (24, 2)]</t>
         </is>
       </c>
     </row>
@@ -2358,19 +2358,19 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F57" t="n">
         <v>26</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>0.654</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 21), (2, 5), (3, 7), (4, 4), (5, 9), (6, 21), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 7), (13, 13), (14, 21), (15, 15), (16, 16), (17, 21), (18, 18), (19, 19), (20, 20), (21, 9), (22, 22), (23, 23), (24, 24), (25, 25)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 14), (11, 21), (12, 24), (13, 20), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25)]</t>
         </is>
       </c>
     </row>
@@ -2392,19 +2392,19 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F58" t="n">
         <v>26</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0.346</t>
+          <t>0.885</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 21), (2, 21), (3, 24), (4, 21), (5, 5), (6, 21), (7, 7), (8, 8), (9, 9), (10, 9), (11, 24), (12, 14), (13, 21), (14, 21), (15, 7), (16, 16), (17, 21), (18, 18), (19, 7), (20, 24), (21, 21), (22, 5), (23, 21), (24, 5), (25, 25)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 1), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 3), (14, 14), (15, 15), (16, 16), (17, 24), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25)]</t>
         </is>
       </c>
     </row>
@@ -2426,19 +2426,19 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F59" t="n">
         <v>26</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>0.346</t>
+          <t>0.654</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 21), (2, 21), (3, 21), (4, 21), (5, 9), (6, 21), (7, 21), (8, 8), (9, 21), (10, 5), (11, 11), (12, 21), (13, 21), (14, 14), (15, 15), (16, 16), (17, 21), (18, 18), (19, 16), (20, 21), (21, 21), (22, 16), (23, 9), (24, 21), (25, 25)]</t>
+          <t>[(0, 0), (1, 21), (2, 1), (3, 16), (4, 4), (5, 5), (6, 16), (7, 7), (8, 8), (9, 14), (10, 18), (11, 11), (12, 18), (13, 18), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 16)]</t>
         </is>
       </c>
     </row>
@@ -2460,19 +2460,19 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>26</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>0.231</t>
+          <t>0.269</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>[(0, 24), (1, 21), (2, 21), (3, 25), (4, 5), (5, 21), (6, 21), (7, 7), (8, 9), (9, 21), (10, 21), (11, 14), (12, 9), (13, 21), (14, 21), (15, 1), (16, 16), (17, 17), (18, 18), (19, 14), (20, 14), (21, 21), (22, 21), (23, 21), (24, 24), (25, 21)]</t>
+          <t>[(0, 18), (1, 21), (2, 2), (3, 15), (4, 24), (5, 8), (6, 18), (7, 7), (8, 18), (9, 6), (10, 21), (11, 8), (12, 23), (13, 18), (14, 18), (15, 15), (16, 21), (17, 18), (18, 18), (19, 18), (20, 20), (21, 24), (22, 8), (23, 23), (24, 24), (25, 12)]</t>
         </is>
       </c>
     </row>
@@ -2494,19 +2494,19 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>26</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>0.038</t>
+          <t>0.231</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>[(0, 24), (1, 21), (2, 21), (3, 21), (4, 21), (5, 21), (6, 21), (7, 21), (8, 21), (9, 21), (10, 21), (11, 7), (12, 9), (13, 9), (14, 21), (15, 21), (16, 21), (17, 21), (18, 3), (19, 14), (20, 21), (21, 21), (22, 21), (23, 21), (24, 21), (25, 21)]</t>
+          <t>[(0, 16), (1, 18), (2, 2), (3, 18), (4, 4), (5, 24), (6, 8), (7, 20), (8, 18), (9, 9), (10, 24), (11, 11), (12, 24), (13, 18), (14, 21), (15, 9), (16, 18), (17, 17), (18, 18), (19, 8), (20, 8), (21, 18), (22, 18), (23, 18), (24, 18), (25, 24)]</t>
         </is>
       </c>
     </row>
@@ -2562,19 +2562,19 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>4</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 2), (3, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 0)]</t>
         </is>
       </c>
     </row>
@@ -2596,19 +2596,19 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>4</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 2), (3, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3)]</t>
         </is>
       </c>
     </row>
@@ -2630,19 +2630,19 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>4</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 0), (3, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 0), (3, 0)]</t>
         </is>
       </c>
     </row>
@@ -2664,19 +2664,19 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>4</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 0), (3, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3)]</t>
         </is>
       </c>
     </row>
@@ -2766,19 +2766,19 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>8</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 0), (3, 3), (4, 4), (5, 5), (6, 1), (7, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7)]</t>
         </is>
       </c>
     </row>
@@ -2800,19 +2800,19 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>8</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 0), (3, 3), (4, 4), (5, 5), (6, 0), (7, 7)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7)]</t>
         </is>
       </c>
     </row>
@@ -2834,19 +2834,19 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>8</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 7), (3, 3), (4, 5), (5, 4), (6, 1), (7, 2)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7)]</t>
         </is>
       </c>
     </row>
@@ -2868,19 +2868,19 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>8</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>0.375</t>
+          <t>0.625</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 2), (2, 0), (3, 1), (4, 4), (5, 5), (6, 1), (7, 2)]</t>
+          <t>[(0, 2), (1, 1), (2, 2), (3, 0), (4, 4), (5, 5), (6, 6), (7, 2)]</t>
         </is>
       </c>
     </row>
@@ -2902,19 +2902,19 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>8</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.375</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 0), (3, 0), (4, 0), (5, 5), (6, 1), (7, 2)]</t>
+          <t>[(0, 1), (1, 2), (2, 2), (3, 2), (4, 4), (5, 5), (6, 2), (7, 2)]</t>
         </is>
       </c>
     </row>
@@ -2970,19 +2970,19 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
         <v>10</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 5), (8, 8), (9, 9)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9)]</t>
         </is>
       </c>
     </row>
@@ -3004,19 +3004,19 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
         <v>10</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>0.700</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 1), (5, 5), (6, 6), (7, 5), (8, 5), (9, 9)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9)]</t>
         </is>
       </c>
     </row>
@@ -3038,19 +3038,19 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>10</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>0.700</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 6), (5, 5), (6, 6), (7, 5), (8, 6), (9, 9)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 9), (4, 7), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9)]</t>
         </is>
       </c>
     </row>
@@ -3072,19 +3072,19 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>10</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>0.300</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>[(0, 7), (1, 5), (2, 7), (3, 3), (4, 3), (5, 5), (6, 6), (7, 5), (8, 6), (9, 6)]</t>
+          <t>[(0, 2), (1, 5), (2, 8), (3, 9), (4, 4), (5, 5), (6, 6), (7, 9), (8, 8), (9, 9)]</t>
         </is>
       </c>
     </row>
@@ -3106,19 +3106,19 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>10</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>0.300</t>
+          <t>0.200</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 6), (2, 6), (3, 5), (4, 3), (5, 5), (6, 6), (7, 3), (8, 3), (9, 6)]</t>
+          <t>[(0, 6), (1, 7), (2, 8), (3, 5), (4, 5), (5, 7), (6, 8), (7, 7), (8, 6), (9, 9)]</t>
         </is>
       </c>
     </row>
@@ -3174,19 +3174,19 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>9</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.444</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 6), (2, 0), (3, 0), (4, 0), (5, 7), (6, 6), (7, 7), (8, 0)]</t>
+          <t>[(0, 0), (1, 1), (2, 1), (3, 0), (4, 5), (5, 5), (6, 6), (7, 1), (8, 0)]</t>
         </is>
       </c>
     </row>
@@ -3208,19 +3208,19 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>9</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.222</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 0), (2, 0), (3, 0), (4, 6), (5, 7), (6, 6), (7, 7), (8, 7)]</t>
+          <t>[(0, 0), (1, 1), (2, 1), (3, 1), (4, 5), (5, 1), (6, 2), (7, 0), (8, 0)]</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>[(0, 6), (1, 0), (2, 7), (3, 6), (4, 0), (5, 7), (6, 0), (7, 7), (8, 0)]</t>
+          <t>[(0, 0), (1, 2), (2, 1), (3, 1), (4, 1), (5, 2), (6, 1), (7, 5), (8, 6)]</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>[(0, 6), (1, 1), (2, 0), (3, 0), (4, 0), (5, 7), (6, 0), (7, 7), (8, 7)]</t>
+          <t>[(0, 0), (1, 0), (2, 1), (3, 1), (4, 1), (5, 5), (6, 1), (7, 1), (8, 6)]</t>
         </is>
       </c>
     </row>
@@ -3310,19 +3310,19 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
         <v>9</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>0.111</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>[(0, 7), (1, 7), (2, 7), (3, 0), (4, 7), (5, 0), (6, 0), (7, 7), (8, 7)]</t>
+          <t>[(0, 2), (1, 0), (2, 1), (3, 1), (4, 5), (5, 0), (6, 1), (7, 5), (8, 0)]</t>
         </is>
       </c>
     </row>
@@ -3378,19 +3378,19 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F87" t="n">
         <v>12</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.917</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 8), (2, 2), (3, 7), (4, 4), (5, 5), (6, 9), (7, 7), (8, 8), (9, 11), (10, 11), (11, 11)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 9), (11, 11)]</t>
         </is>
       </c>
     </row>
@@ -3412,19 +3412,19 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F88" t="n">
         <v>12</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>0.583</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 1), (2, 2), (3, 3), (4, 4), (5, 8), (6, 4), (7, 7), (8, 8), (9, 11), (10, 11), (11, 11)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 5), (4, 4), (5, 11), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11)]</t>
         </is>
       </c>
     </row>
@@ -3446,19 +3446,19 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>12</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.333</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>[(0, 11), (1, 8), (2, 7), (3, 8), (4, 4), (5, 5), (6, 3), (7, 7), (8, 8), (9, 9), (10, 11), (11, 11)]</t>
+          <t>[(0, 11), (1, 1), (2, 11), (3, 11), (4, 11), (5, 11), (6, 9), (7, 11), (8, 8), (9, 9), (10, 8), (11, 11)]</t>
         </is>
       </c>
     </row>
@@ -3480,19 +3480,19 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>12</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>0.417</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 8), (2, 4), (3, 3), (4, 4), (5, 5), (6, 11), (7, 5), (8, 8), (9, 8), (10, 0), (11, 11)]</t>
+          <t>[(0, 0), (1, 11), (2, 2), (3, 5), (4, 11), (5, 5), (6, 11), (7, 11), (8, 8), (9, 11), (10, 10), (11, 11)]</t>
         </is>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 5), (2, 8), (3, 8), (4, 8), (5, 8), (6, 0), (7, 11), (8, 11), (9, 3), (10, 11), (11, 11)]</t>
+          <t>[(0, 11), (1, 6), (2, 11), (3, 11), (4, 11), (5, 11), (6, 11), (7, 11), (8, 9), (9, 11), (10, 11), (11, 11)]</t>
         </is>
       </c>
     </row>
@@ -3582,19 +3582,19 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F93" t="n">
         <v>23</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>0.739</t>
+          <t>0.913</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 15), (9, 9), (10, 10), (11, 6), (12, 12), (13, 22), (14, 8), (15, 10), (16, 9), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 10), (12, 12), (13, 13), (14, 14), (15, 15), (16, 22), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22)]</t>
         </is>
       </c>
     </row>
@@ -3616,19 +3616,19 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F94" t="n">
         <v>23</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>0.696</t>
+          <t>0.826</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>[(0, 10), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 18), (12, 6), (13, 13), (14, 14), (15, 10), (16, 9), (17, 6), (18, 18), (19, 13), (20, 20), (21, 21), (22, 22)]</t>
+          <t>[(0, 20), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 10), (12, 12), (13, 13), (14, 14), (15, 6), (16, 22), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22)]</t>
         </is>
       </c>
     </row>
@@ -3650,19 +3650,19 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F95" t="n">
         <v>23</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>0.304</t>
+          <t>0.609</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>[(0, 8), (1, 1), (2, 3), (3, 19), (4, 21), (5, 5), (6, 6), (7, 18), (8, 10), (9, 18), (10, 10), (11, 6), (12, 12), (13, 21), (14, 18), (15, 10), (16, 9), (17, 8), (18, 10), (19, 18), (20, 11), (21, 21), (22, 22)]</t>
+          <t>[(0, 0), (1, 1), (2, 22), (3, 3), (4, 4), (5, 5), (6, 6), (7, 10), (8, 22), (9, 6), (10, 10), (11, 4), (12, 12), (13, 13), (14, 14), (15, 22), (16, 6), (17, 4), (18, 22), (19, 19), (20, 20), (21, 21), (22, 22)]</t>
         </is>
       </c>
     </row>
@@ -3684,19 +3684,19 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F96" t="n">
         <v>23</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>0.261</t>
+          <t>0.565</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>[(0, 9), (1, 1), (2, 18), (3, 10), (4, 2), (5, 10), (6, 6), (7, 10), (8, 8), (9, 9), (10, 18), (11, 10), (12, 6), (13, 21), (14, 21), (15, 18), (16, 10), (17, 11), (18, 18), (19, 6), (20, 12), (21, 18), (22, 22)]</t>
+          <t>[(0, 20), (1, 1), (2, 10), (3, 17), (4, 4), (5, 5), (6, 6), (7, 4), (8, 6), (9, 9), (10, 10), (11, 6), (12, 12), (13, 13), (14, 14), (15, 22), (16, 6), (17, 20), (18, 18), (19, 19), (20, 20), (21, 6), (22, 22)]</t>
         </is>
       </c>
     </row>
@@ -3718,19 +3718,19 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>23</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>0.087</t>
+          <t>0.130</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>[(0, 17), (1, 1), (2, 7), (3, 18), (4, 6), (5, 10), (6, 18), (7, 18), (8, 6), (9, 11), (10, 10), (11, 18), (12, 10), (13, 7), (14, 6), (15, 18), (16, 6), (17, 18), (18, 10), (19, 10), (20, 21), (21, 18), (22, 18)]</t>
+          <t>[(0, 10), (1, 1), (2, 12), (3, 13), (4, 4), (5, 20), (6, 12), (7, 6), (8, 13), (9, 22), (10, 19), (11, 4), (12, 18), (13, 12), (14, 6), (15, 6), (16, 4), (17, 10), (18, 9), (19, 19), (20, 19), (21, 12), (22, 6)]</t>
         </is>
       </c>
     </row>
@@ -3786,19 +3786,19 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F99" t="n">
         <v>25</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>0.840</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 24), (5, 0), (6, 6), (7, 7), (8, 8), (9, 9), (10, 14), (11, 11), (12, 12), (13, 23), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 18), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
         </is>
       </c>
     </row>
@@ -3820,19 +3820,19 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F100" t="n">
         <v>25</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 7), (2, 2), (3, 3), (4, 24), (5, 14), (6, 6), (7, 7), (8, 8), (9, 9), (10, 0), (11, 11), (12, 12), (13, 0), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 4), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
         </is>
       </c>
     </row>
@@ -3854,19 +3854,19 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F101" t="n">
         <v>25</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>0.440</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 7), (2, 2), (3, 3), (4, 16), (5, 14), (6, 6), (7, 24), (8, 19), (9, 9), (10, 14), (11, 20), (12, 11), (13, 23), (14, 14), (15, 23), (16, 19), (17, 7), (18, 0), (19, 24), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 18), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 19), (11, 11), (12, 7), (13, 9), (14, 14), (15, 15), (16, 16), (17, 7), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
         </is>
       </c>
     </row>
@@ -3888,19 +3888,19 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F102" t="n">
         <v>25</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>0.280</t>
+          <t>0.640</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>[(0, 24), (1, 19), (2, 2), (3, 24), (4, 24), (5, 14), (6, 20), (7, 24), (8, 23), (9, 24), (10, 19), (11, 11), (12, 20), (13, 7), (14, 24), (15, 19), (16, 0), (17, 17), (18, 9), (19, 19), (20, 20), (21, 24), (22, 22), (23, 7), (24, 24)]</t>
+          <t>[(0, 0), (1, 11), (2, 2), (3, 3), (4, 4), (5, 18), (6, 3), (7, 7), (8, 5), (9, 9), (10, 19), (11, 11), (12, 12), (13, 11), (14, 0), (15, 15), (16, 16), (17, 17), (18, 0), (19, 19), (20, 18), (21, 21), (22, 22), (23, 23), (24, 24)]</t>
         </is>
       </c>
     </row>
@@ -3922,19 +3922,19 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F103" t="n">
         <v>25</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>0.160</t>
+          <t>0.200</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 14), (2, 24), (3, 14), (4, 24), (5, 14), (6, 19), (7, 24), (8, 7), (9, 24), (10, 14), (11, 19), (12, 19), (13, 0), (14, 14), (15, 24), (16, 24), (17, 14), (18, 24), (19, 19), (20, 0), (21, 24), (22, 0), (23, 23), (24, 24)]</t>
+          <t>[(0, 0), (1, 24), (2, 16), (3, 3), (4, 14), (5, 18), (6, 21), (7, 7), (8, 9), (9, 7), (10, 19), (11, 7), (12, 5), (13, 18), (14, 3), (15, 19), (16, 7), (17, 7), (18, 18), (19, 5), (20, 19), (21, 19), (22, 16), (23, 23), (24, 7)]</t>
         </is>
       </c>
     </row>
@@ -3990,19 +3990,19 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="F105" t="n">
         <v>78</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>0.590</t>
+          <t>0.974</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 75), (2, 2), (3, 3), (4, 20), (5, 5), (6, 6), (7, 7), (8, 8), (9, 75), (10, 10), (11, 6), (12, 75), (13, 13), (14, 14), (15, 72), (16, 16), (17, 17), (18, 18), (19, 11), (20, 31), (21, 21), (22, 74), (23, 66), (24, 70), (25, 53), (26, 26), (27, 27), (28, 42), (29, 76), (30, 19), (31, 31), (32, 69), (33, 70), (34, 75), (35, 35), (36, 70), (37, 37), (38, 38), (39, 73), (40, 40), (41, 41), (42, 43), (43, 43), (44, 44), (45, 57), (46, 46), (47, 47), (48, 48), (49, 69), (50, 75), (51, 51), (52, 75), (53, 53), (54, 54), (55, 55), (56, 69), (57, 75), (58, 58), (59, 59), (60, 60), (61, 59), (62, 42), (63, 64), (64, 64), (65, 65), (66, 66), (67, 70), (68, 68), (69, 69), (70, 70), (71, 71), (72, 72), (73, 73), (74, 74), (75, 75), (76, 76), (77, 75)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 24), (25, 25), (26, 26), (27, 27), (28, 28), (29, 29), (30, 30), (31, 31), (32, 32), (33, 33), (34, 34), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39), (40, 40), (41, 41), (42, 42), (43, 43), (44, 44), (45, 45), (46, 46), (47, 47), (48, 48), (49, 49), (50, 46), (51, 51), (52, 52), (53, 53), (54, 54), (55, 55), (56, 56), (57, 57), (58, 58), (59, 59), (60, 60), (61, 61), (62, 62), (63, 63), (64, 64), (65, 65), (66, 66), (67, 67), (68, 68), (69, 69), (70, 70), (71, 71), (72, 72), (73, 73), (74, 74), (75, 75), (76, 76), (77, 38)]</t>
         </is>
       </c>
     </row>
@@ -4024,19 +4024,19 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F106" t="n">
         <v>78</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 13), (4, 4), (5, 51), (6, 6), (7, 76), (8, 58), (9, 75), (10, 0), (11, 11), (12, 64), (13, 13), (14, 53), (15, 51), (16, 16), (17, 75), (18, 75), (19, 13), (20, 20), (21, 51), (22, 33), (23, 27), (24, 70), (25, 41), (26, 71), (27, 69), (28, 64), (29, 76), (30, 75), (31, 31), (32, 70), (33, 70), (34, 75), (35, 35), (36, 36), (37, 37), (38, 38), (39, 76), (40, 40), (41, 41), (42, 43), (43, 31), (44, 44), (45, 13), (46, 46), (47, 47), (48, 48), (49, 69), (50, 50), (51, 43), (52, 52), (53, 53), (54, 54), (55, 55), (56, 56), (57, 75), (58, 70), (59, 59), (60, 60), (61, 61), (62, 39), (63, 63), (64, 64), (65, 75), (66, 66), (67, 70), (68, 75), (69, 69), (70, 70), (71, 71), (72, 72), (73, 73), (74, 74), (75, 70), (76, 76), (77, 75)]</t>
+          <t>[(0, 0), (1, 18), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 11), (9, 9), (10, 10), (11, 11), (12, 38), (13, 13), (14, 10), (15, 18), (16, 16), (17, 17), (18, 55), (19, 18), (20, 20), (21, 21), (22, 22), (23, 33), (24, 18), (25, 25), (26, 75), (27, 27), (28, 28), (29, 29), (30, 30), (31, 28), (32, 52), (33, 33), (34, 45), (35, 35), (36, 33), (37, 37), (38, 38), (39, 39), (40, 40), (41, 41), (42, 42), (43, 75), (44, 44), (45, 59), (46, 46), (47, 59), (48, 52), (49, 49), (50, 50), (51, 51), (52, 52), (53, 53), (54, 54), (55, 55), (56, 56), (57, 75), (58, 75), (59, 59), (60, 60), (61, 61), (62, 62), (63, 63), (64, 73), (65, 65), (66, 66), (67, 67), (68, 68), (69, 69), (70, 70), (71, 55), (72, 72), (73, 73), (74, 74), (75, 75), (76, 76), (77, 77)]</t>
         </is>
       </c>
     </row>
@@ -4058,19 +4058,19 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F107" t="n">
         <v>78</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>0.244</t>
+          <t>0.385</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>[(0, 31), (1, 75), (2, 54), (3, 3), (4, 75), (5, 56), (6, 6), (7, 13), (8, 70), (9, 75), (10, 75), (11, 64), (12, 76), (13, 65), (14, 14), (15, 15), (16, 74), (17, 66), (18, 75), (19, 42), (20, 20), (21, 69), (22, 64), (23, 59), (24, 44), (25, 31), (26, 56), (27, 20), (28, 75), (29, 68), (30, 73), (31, 38), (32, 51), (33, 70), (34, 66), (35, 56), (36, 65), (37, 37), (38, 75), (39, 70), (40, 40), (41, 70), (42, 64), (43, 70), (44, 55), (45, 13), (46, 56), (47, 47), (48, 48), (49, 70), (50, 31), (51, 31), (52, 75), (53, 72), (54, 70), (55, 43), (56, 43), (57, 28), (58, 70), (59, 59), (60, 60), (61, 61), (62, 31), (63, 74), (64, 31), (65, 75), (66, 43), (67, 67), (68, 76), (69, 69), (70, 70), (71, 75), (72, 72), (73, 73), (74, 74), (75, 75), (76, 53), (77, 75)]</t>
+          <t>[(0, 0), (1, 18), (2, 18), (3, 13), (4, 4), (5, 5), (6, 11), (7, 76), (8, 11), (9, 11), (10, 75), (11, 11), (12, 75), (13, 28), (14, 22), (15, 15), (16, 18), (17, 38), (18, 55), (19, 28), (20, 20), (21, 28), (22, 22), (23, 23), (24, 20), (25, 24), (26, 26), (27, 17), (28, 28), (29, 58), (30, 75), (31, 75), (32, 71), (33, 33), (34, 59), (35, 61), (36, 28), (37, 37), (38, 75), (39, 59), (40, 40), (41, 55), (42, 76), (43, 73), (44, 44), (45, 75), (46, 46), (47, 47), (48, 48), (49, 49), (50, 59), (51, 51), (52, 33), (53, 53), (54, 55), (55, 55), (56, 39), (57, 75), (58, 10), (59, 59), (60, 60), (61, 59), (62, 68), (63, 63), (64, 72), (65, 65), (66, 65), (67, 67), (68, 72), (69, 69), (70, 75), (71, 55), (72, 72), (73, 73), (74, 75), (75, 75), (76, 64), (77, 38)]</t>
         </is>
       </c>
     </row>
@@ -4092,19 +4092,19 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F108" t="n">
         <v>78</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>0.167</t>
+          <t>0.205</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>[(0, 75), (1, 69), (2, 76), (3, 53), (4, 31), (5, 69), (6, 69), (7, 74), (8, 31), (9, 75), (10, 31), (11, 31), (12, 75), (13, 38), (14, 14), (15, 31), (16, 76), (17, 31), (18, 75), (19, 19), (20, 20), (21, 21), (22, 75), (23, 59), (24, 31), (25, 31), (26, 70), (27, 64), (28, 75), (29, 70), (30, 75), (31, 31), (32, 75), (33, 33), (34, 31), (35, 31), (36, 72), (37, 43), (38, 43), (39, 72), (40, 75), (41, 56), (42, 75), (43, 43), (44, 44), (45, 75), (46, 37), (47, 70), (48, 31), (49, 70), (50, 53), (51, 31), (52, 75), (53, 53), (54, 38), (55, 53), (56, 31), (57, 75), (58, 43), (59, 60), (60, 64), (61, 75), (62, 75), (63, 75), (64, 53), (65, 53), (66, 31), (67, 67), (68, 31), (69, 64), (70, 31), (71, 31), (72, 72), (73, 31), (74, 75), (75, 75), (76, 76), (77, 75)]</t>
+          <t>[(0, 0), (1, 46), (2, 1), (3, 38), (4, 4), (5, 11), (6, 11), (7, 46), (8, 11), (9, 9), (10, 18), (11, 11), (12, 20), (13, 38), (14, 14), (15, 55), (16, 57), (17, 38), (18, 55), (19, 17), (20, 20), (21, 20), (22, 18), (23, 57), (24, 68), (25, 38), (26, 55), (27, 20), (28, 55), (29, 45), (30, 28), (31, 75), (32, 55), (33, 17), (34, 75), (35, 38), (36, 72), (37, 45), (38, 55), (39, 75), (40, 75), (41, 28), (42, 59), (43, 43), (44, 43), (45, 59), (46, 38), (47, 47), (48, 73), (49, 75), (50, 73), (51, 46), (52, 70), (53, 73), (54, 55), (55, 55), (56, 56), (57, 1), (58, 73), (59, 59), (60, 60), (61, 61), (62, 75), (63, 72), (64, 73), (65, 70), (66, 73), (67, 72), (68, 38), (69, 38), (70, 72), (71, 71), (72, 43), (73, 73), (74, 75), (75, 75), (76, 55), (77, 73)]</t>
         </is>
       </c>
     </row>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>[(0, 28), (1, 31), (2, 31), (3, 47), (4, 4), (5, 74), (6, 75), (7, 75), (8, 31), (9, 75), (10, 43), (11, 38), (12, 76), (13, 70), (14, 70), (15, 28), (16, 31), (17, 31), (18, 31), (19, 75), (20, 75), (21, 75), (22, 31), (23, 59), (24, 41), (25, 38), (26, 75), (27, 38), (28, 38), (29, 53), (30, 64), (31, 31), (32, 75), (33, 75), (34, 31), (35, 75), (36, 72), (37, 37), (38, 77), (39, 70), (40, 72), (41, 38), (42, 48), (43, 75), (44, 37), (45, 64), (46, 70), (47, 47), (48, 31), (49, 47), (50, 75), (51, 53), (52, 75), (53, 53), (54, 53), (55, 31), (56, 31), (57, 31), (58, 53), (59, 31), (60, 75), (61, 31), (62, 75), (63, 31), (64, 37), (65, 59), (66, 31), (67, 64), (68, 75), (69, 37), (70, 43), (71, 38), (72, 75), (73, 31), (74, 31), (75, 37), (76, 37), (77, 75)]</t>
+          <t>[(0, 11), (1, 18), (2, 75), (3, 20), (4, 11), (5, 5), (6, 11), (7, 75), (8, 11), (9, 11), (10, 38), (11, 11), (12, 52), (13, 68), (14, 28), (15, 75), (16, 38), (17, 38), (18, 38), (19, 72), (20, 38), (21, 55), (22, 22), (23, 18), (24, 72), (25, 28), (26, 26), (27, 75), (28, 38), (29, 65), (30, 55), (31, 55), (32, 3), (33, 20), (34, 55), (35, 28), (36, 22), (37, 73), (38, 72), (39, 70), (40, 55), (41, 68), (42, 70), (43, 55), (44, 75), (45, 55), (46, 75), (47, 59), (48, 70), (49, 72), (50, 55), (51, 59), (52, 72), (53, 59), (54, 59), (55, 72), (56, 55), (57, 71), (58, 55), (59, 70), (60, 55), (61, 55), (62, 55), (63, 73), (64, 73), (65, 73), (66, 66), (67, 72), (68, 59), (69, 72), (70, 55), (71, 69), (72, 65), (73, 56), (74, 73), (75, 55), (76, 70), (77, 55)]</t>
         </is>
       </c>
     </row>
@@ -4194,19 +4194,19 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F111" t="n">
         <v>14</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 10), (2, 2), (3, 3), (4, 4), (5, 5), (6, 8), (7, 7), (8, 8), (9, 9), (10, 10), (11, 7), (12, 0), (13, 2)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 12), (12, 12), (13, 13)]</t>
         </is>
       </c>
     </row>
@@ -4228,19 +4228,19 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F112" t="n">
         <v>14</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>0.571</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 10), (2, 2), (3, 3), (4, 10), (5, 5), (6, 8), (7, 7), (8, 10), (9, 9), (10, 10), (11, 8), (12, 10), (13, 13)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 9), (12, 12), (13, 5)]</t>
         </is>
       </c>
     </row>
@@ -4262,19 +4262,19 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F113" t="n">
         <v>14</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>0.571</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 8), (2, 2), (3, 3), (4, 10), (5, 5), (6, 6), (7, 7), (8, 10), (9, 9), (10, 10), (11, 2), (12, 3), (13, 2)]</t>
+          <t>[(0, 0), (1, 7), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13)]</t>
         </is>
       </c>
     </row>
@@ -4296,19 +4296,19 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F114" t="n">
         <v>14</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>0.357</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>[(0, 3), (1, 10), (2, 10), (3, 3), (4, 3), (5, 5), (6, 12), (7, 10), (8, 8), (9, 9), (10, 10), (11, 8), (12, 10), (13, 10)]</t>
+          <t>[(0, 3), (1, 4), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 10), (9, 9), (10, 10), (11, 12), (12, 7), (13, 5)]</t>
         </is>
       </c>
     </row>
@@ -4330,19 +4330,19 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F115" t="n">
         <v>14</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>0.143</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>[(0, 10), (1, 10), (2, 10), (3, 3), (4, 10), (5, 10), (6, 7), (7, 0), (8, 10), (9, 9), (10, 3), (11, 7), (12, 3), (13, 8)]</t>
+          <t>[(0, 12), (1, 9), (2, 2), (3, 3), (4, 10), (5, 2), (6, 6), (7, 7), (8, 4), (9, 9), (10, 10), (11, 12), (12, 7), (13, 13)]</t>
         </is>
       </c>
     </row>
@@ -4398,19 +4398,19 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F117" t="n">
         <v>17</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>0.588</t>
+          <t>0.882</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 12), (2, 12), (3, 3), (4, 4), (5, 5), (6, 16), (7, 7), (8, 8), (9, 10), (10, 10), (11, 12), (12, 12), (13, 12), (14, 14), (15, 15), (16, 14)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 4), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 10)]</t>
         </is>
       </c>
     </row>
@@ -4444,7 +4444,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 16), (2, 2), (3, 3), (4, 4), (5, 5), (6, 2), (7, 7), (8, 8), (9, 9), (10, 10), (11, 12), (12, 12), (13, 13), (14, 14), (15, 15), (16, 12)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 12), (7, 7), (8, 8), (9, 1), (10, 5), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 5)]</t>
         </is>
       </c>
     </row>
@@ -4466,19 +4466,19 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F119" t="n">
         <v>17</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>0.529</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 16), (2, 10), (3, 3), (4, 4), (5, 16), (6, 6), (7, 16), (8, 12), (9, 16), (10, 10), (11, 11), (12, 12), (13, 13), (14, 12), (15, 16), (16, 16)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 0), (7, 7), (8, 8), (9, 9), (10, 1), (11, 11), (12, 12), (13, 13), (14, 14), (15, 5), (16, 11)]</t>
         </is>
       </c>
     </row>
@@ -4500,19 +4500,19 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F120" t="n">
         <v>17</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>0.235</t>
+          <t>0.294</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>[(0, 12), (1, 12), (2, 12), (3, 10), (4, 12), (5, 16), (6, 6), (7, 14), (8, 8), (9, 12), (10, 10), (11, 5), (12, 12), (13, 16), (14, 6), (15, 10), (16, 12)]</t>
+          <t>[(0, 0), (1, 5), (2, 2), (3, 11), (4, 8), (5, 5), (6, 12), (7, 11), (8, 5), (9, 1), (10, 5), (11, 9), (12, 12), (13, 8), (14, 14), (15, 12), (16, 9)]</t>
         </is>
       </c>
     </row>
@@ -4534,19 +4534,19 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F121" t="n">
         <v>17</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>0.118</t>
+          <t>0.235</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 14), (2, 10), (3, 10), (4, 5), (5, 10), (6, 16), (7, 10), (8, 12), (9, 10), (10, 10), (11, 16), (12, 16), (13, 12), (14, 10), (15, 10), (16, 16)]</t>
+          <t>[(0, 0), (1, 5), (2, 5), (3, 9), (4, 4), (5, 5), (6, 12), (7, 5), (8, 12), (9, 8), (10, 8), (11, 4), (12, 12), (13, 2), (14, 5), (15, 14), (16, 11)]</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 6), (9, 3), (10, 10), (11, 11), (12, 15), (13, 13), (14, 14), (15, 15), (16, 16)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 2), (7, 7), (8, 6), (9, 2), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16)]</t>
         </is>
       </c>
     </row>
@@ -4636,19 +4636,19 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F124" t="n">
         <v>17</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>0.529</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>[(0, 0), (1, 6), (2, 2), (3, 3), (4, 4), (5, 5), (6, 2), (7, 7), (8, 6), (9, 10), (10, 10), (11, 11), (12, 3), (13, 2), (14, 14), (15, 6), (16, 10)]</t>
+          <t>[(0, 3), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 4), (10, 10), (11, 11), (12, 2), (13, 13), (14, 14), (15, 3), (16, 16)]</t>
         </is>
       </c>
     </row>
@@ -4670,19 +4670,19 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F125" t="n">
         <v>17</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>0.235</t>
+          <t>0.529</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>[(0, 10), (1, 6), (2, 2), (3, 14), (4, 4), (5, 3), (6, 14), (7, 11), (8, 14), (9, 3), (10, 14), (11, 14), (12, 6), (13, 3), (14, 14), (15, 15), (16, 6)]</t>
+          <t>[(0, 0), (1, 3), (2, 2), (3, 3), (4, 4), (5, 5), (6, 2), (7, 7), (8, 5), (9, 10), (10, 3), (11, 11), (12, 12), (13, 13), (14, 2), (15, 4), (16, 2)]</t>
         </is>
       </c>
     </row>
@@ -4704,19 +4704,19 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F126" t="n">
         <v>17</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>0.118</t>
+          <t>0.412</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 6), (2, 2), (3, 2), (4, 6), (5, 6), (6, 2), (7, 6), (8, 2), (9, 6), (10, 2), (11, 2), (12, 3), (13, 14), (14, 14), (15, 14), (16, 2)]</t>
+          <t>[(0, 10), (1, 1), (2, 2), (3, 3), (4, 3), (5, 5), (6, 2), (7, 10), (8, 4), (9, 5), (10, 2), (11, 11), (12, 3), (13, 13), (14, 14), (15, 5), (16, 6)]</t>
         </is>
       </c>
     </row>
@@ -4738,19 +4738,19 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F127" t="n">
         <v>17</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>0.059</t>
+          <t>0.176</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>[(0, 14), (1, 2), (2, 2), (3, 2), (4, 14), (5, 14), (6, 2), (7, 14), (8, 2), (9, 3), (10, 14), (11, 2), (12, 14), (13, 2), (14, 2), (15, 2), (16, 6)]</t>
+          <t>[(0, 11), (1, 14), (2, 2), (3, 2), (4, 3), (5, 2), (6, 2), (7, 11), (8, 14), (9, 4), (10, 3), (11, 2), (12, 3), (13, 13), (14, 3), (15, 3), (16, 16)]</t>
         </is>
       </c>
     </row>
@@ -4806,19 +4806,19 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F129" t="n">
         <v>19</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>[(0, 3), (1, 1), (2, 14), (3, 3), (4, 1), (5, 3), (6, 6), (7, 7), (8, 8), (9, 9), (10, 3), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 3)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18)]</t>
         </is>
       </c>
     </row>
@@ -4840,19 +4840,19 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F130" t="n">
         <v>19</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>0.526</t>
+          <t>0.895</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>[(0, 16), (1, 1), (2, 12), (3, 3), (4, 9), (5, 3), (6, 6), (7, 7), (8, 8), (9, 9), (10, 12), (11, 11), (12, 12), (13, 3), (14, 14), (15, 12), (16, 1), (17, 17), (18, 3)]</t>
+          <t>[(0, 0), (1, 1), (2, 1), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 18), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18)]</t>
         </is>
       </c>
     </row>
@@ -4874,19 +4874,19 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F131" t="n">
         <v>19</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>0.158</t>
+          <t>0.632</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>[(0, 3), (1, 12), (2, 15), (3, 3), (4, 3), (5, 14), (6, 12), (7, 12), (8, 12), (9, 12), (10, 12), (11, 3), (12, 12), (13, 1), (14, 12), (15, 12), (16, 12), (17, 17), (18, 12)]</t>
+          <t>[(0, 14), (1, 1), (2, 1), (3, 3), (4, 4), (5, 5), (6, 8), (7, 7), (8, 8), (9, 11), (10, 10), (11, 11), (12, 12), (13, 13), (14, 14), (15, 15), (16, 8), (17, 5), (18, 6)]</t>
         </is>
       </c>
     </row>
@@ -4908,19 +4908,19 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F132" t="n">
         <v>19</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>0.211</t>
+          <t>0.526</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>[(0, 12), (1, 1), (2, 12), (3, 12), (4, 3), (5, 16), (6, 12), (7, 3), (8, 12), (9, 12), (10, 12), (11, 12), (12, 12), (13, 6), (14, 14), (15, 15), (16, 12), (17, 3), (18, 12)]</t>
+          <t>[(0, 5), (1, 1), (2, 1), (3, 3), (4, 4), (5, 8), (6, 1), (7, 14), (8, 8), (9, 1), (10, 10), (11, 11), (12, 12), (13, 1), (14, 14), (15, 15), (16, 16), (17, 5), (18, 1)]</t>
         </is>
       </c>
     </row>
@@ -4942,19 +4942,19 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F133" t="n">
         <v>19</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>0.105</t>
+          <t>0.263</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>[(0, 12), (1, 12), (2, 12), (3, 3), (4, 12), (5, 3), (6, 12), (7, 12), (8, 12), (9, 12), (10, 12), (11, 3), (12, 12), (13, 3), (14, 12), (15, 12), (16, 12), (17, 3), (18, 12)]</t>
+          <t>[(0, 1), (1, 1), (2, 18), (3, 3), (4, 5), (5, 18), (6, 6), (7, 14), (8, 18), (9, 1), (10, 10), (11, 6), (12, 5), (13, 1), (14, 8), (15, 18), (16, 1), (17, 5), (18, 18)]</t>
         </is>
       </c>
     </row>
@@ -5010,19 +5010,19 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F135" t="n">
         <v>41</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>0.488</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>[(0, 29), (1, 24), (2, 29), (3, 29), (4, 11), (5, 5), (6, 6), (7, 21), (8, 6), (9, 29), (10, 10), (11, 11), (12, 12), (13, 13), (14, 17), (15, 11), (16, 29), (17, 17), (18, 35), (19, 24), (20, 29), (21, 21), (22, 22), (23, 11), (24, 24), (25, 29), (26, 29), (27, 27), (28, 11), (29, 29), (30, 30), (31, 31), (32, 21), (33, 11), (34, 11), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39), (40, 40)]</t>
+          <t>[(0, 0), (1, 1), (2, 2), (3, 3), (4, 4), (5, 5), (6, 6), (7, 7), (8, 8), (9, 9), (10, 10), (11, 11), (12, 12), (13, 11), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 21), (22, 22), (23, 23), (24, 11), (25, 29), (26, 26), (27, 27), (28, 11), (29, 29), (30, 30), (31, 31), (32, 11), (33, 33), (34, 34), (35, 35), (36, 36), (37, 37), (38, 38), (39, 39), (40, 40)]</t>
         </is>
       </c>
     </row>
@@ -5044,19 +5044,19 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F136" t="n">
         <v>41</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>0.244</t>
+          <t>0.634</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>[(0, 11), (1, 17), (2, 11), (3, 29), (4, 11), (5, 24), (6, 21), (7, 21), (8, 6), (9, 35), (10, 35), (11, 11), (12, 12), (13, 21), (14, 17), (15, 21), (16, 29), (17, 17), (18, 35), (19, 21), (20, 29), (21, 11), (22, 22), (23, 24), (24, 24), (25, 29), (26, 29), (27, 27), (28, 11), (29, 29), (30, 30), (31, 24), (32, 21), (33, 11), (34, 29), (35, 35), (36, 11), (37, 21), (38, 38), (39, 21), (40, 21)]</t>
+          <t>[(0, 11), (1, 1), (2, 11), (3, 11), (4, 4), (5, 5), (6, 6), (7, 7), (8, 11), (9, 11), (10, 10), (11, 11), (12, 29), (13, 13), (14, 14), (15, 15), (16, 16), (17, 17), (18, 18), (19, 19), (20, 20), (21, 29), (22, 22), (23, 11), (24, 35), (25, 29), (26, 26), (27, 29), (28, 11), (29, 29), (30, 30), (31, 31), (32, 11), (33, 11), (34, 34), (35, 35), (36, 36), (37, 11), (38, 38), (39, 39), (40, 40)]</t>
         </is>
       </c>
     </row>
@@ -5078,19 +5078,19 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F137" t="n">
         <v>41</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>0.244</t>
+          <t>0.488</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>[(0, 17), (1, 1), (2, 17), (3, 29), (4, 4), (5, 5), (6, 6), (7, 7), (8, 35), (9, 29), (10, 24), (11, 11), (12, 29), (13, 24), (14, 21), (15, 24), (16, 35), (17, 24), (18, 35), (19, 24), (20, 29), (21, 21), (22, 24), (23, 21), (24, 35), (25, 29), (26, 17), (27, 24), (28, 29), (29, 29), (30, 24), (31, 31), (32, 21), (33, 21), (34, 35), (35, 35), (36, 24), (37, 21), (38, 11), (39, 22), (40, 29)]</t>
+          <t>[(0, 11), (1, 1), (2, 11), (3, 29), (4, 4), (5, 5), (6, 6), (7, 11), (8, 11), (9, 9), (10, 29), (11, 11), (12, 29), (13, 13), (14, 14), (15, 29), (16, 16), (17, 29), (18, 18), (19, 29), (20, 20), (21, 21), (22, 22), (23, 11), (24, 29), (25, 29), (26, 11), (27, 11), (28, 11), (29, 29), (30, 30), (31, 31), (32, 32), (33, 11), (34, 34), (35, 35), (36, 29), (37, 29), (38, 38), (39, 11), (40, 29)]</t>
         </is>
       </c>
     </row>
@@ -5112,19 +5112,19 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F138" t="n">
         <v>41</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>0.146</t>
+          <t>0.341</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>[(0, 29), (1, 24), (2, 29), (3, 27), (4, 35), (5, 13), (6, 24), (7, 21), (8, 24), (9, 35), (10, 35), (11, 24), (12, 29), (13, 6), (14, 29), (15, 11), (16, 24), (17, 17), (18, 8), (19, 21), (20, 11), (21, 21), (22, 35), (23, 21), (24, 24), (25, 35), (26, 24), (27, 24), (28, 35), (29, 29), (30, 30), (31, 24), (32, 21), (33, 11), (34, 29), (35, 35), (36, 13), (37, 24), (38, 21), (39, 35), (40, 17)]</t>
+          <t>[(0, 29), (1, 1), (2, 2), (3, 29), (4, 29), (5, 11), (6, 11), (7, 7), (8, 11), (9, 11), (10, 10), (11, 11), (12, 11), (13, 13), (14, 11), (15, 29), (16, 16), (17, 17), (18, 18), (19, 11), (20, 20), (21, 21), (22, 11), (23, 11), (24, 11), (25, 11), (26, 11), (27, 29), (28, 29), (29, 11), (30, 29), (31, 31), (32, 32), (33, 29), (34, 11), (35, 35), (36, 29), (37, 11), (38, 29), (39, 11), (40, 29)]</t>
         </is>
       </c>
     </row>
@@ -5146,19 +5146,19 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F139" t="n">
         <v>41</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>0.073</t>
+          <t>0.146</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>[(0, 24), (1, 24), (2, 30), (3, 29), (4, 13), (5, 24), (6, 6), (7, 21), (8, 24), (9, 24), (10, 8), (11, 24), (12, 35), (13, 35), (14, 35), (15, 17), (16, 24), (17, 17), (18, 24), (19, 8), (20, 29), (21, 17), (22, 24), (23, 24), (24, 24), (25, 24), (26, 24), (27, 35), (28, 35), (29, 21), (30, 35), (31, 24), (32, 8), (33, 24), (34, 35), (35, 24), (36, 24), (37, 24), (38, 19), (39, 24), (40, 30)]</t>
+          <t>[(0, 11), (1, 29), (2, 29), (3, 29), (4, 16), (5, 5), (6, 35), (7, 11), (8, 18), (9, 35), (10, 22), (11, 11), (12, 5), (13, 11), (14, 17), (15, 5), (16, 16), (17, 11), (18, 29), (19, 29), (20, 11), (21, 21), (22, 22), (23, 35), (24, 11), (25, 29), (26, 29), (27, 29), (28, 29), (29, 29), (30, 29), (31, 11), (32, 5), (33, 29), (34, 11), (35, 11), (36, 5), (37, 11), (38, 35), (39, 18), (40, 11)]</t>
         </is>
       </c>
     </row>

</xml_diff>